<commit_message>
add insert with 10M rows result
</commit_message>
<xml_diff>
--- a/tests/results/vm-results.xlsx
+++ b/tests/results/vm-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="20180" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="20180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NUMBERS" sheetId="3" r:id="rId1"/>
@@ -559,28 +559,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.283075026892407</c:v>
+                  <c:v>0.272750546093145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.362403600651504</c:v>
+                  <c:v>0.354725091704294</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.409526191922477</c:v>
+                  <c:v>0.399676633913056</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.413894602204329</c:v>
+                  <c:v>0.535724474603577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.444899430425951</c:v>
+                  <c:v>0.539497772251148</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.435648901303029</c:v>
+                  <c:v>0.506676066214847</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.152341593116038</c:v>
+                  <c:v>0.232460195576934</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.171523378796933</c:v>
+                  <c:v>0.17321739692286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,28 +670,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.850672355576037</c:v>
+                  <c:v>0.817434894795387</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.037487483379165</c:v>
+                  <c:v>0.981897436270829</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.051806915558913</c:v>
+                  <c:v>1.171880349024415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.970587686437515</c:v>
+                  <c:v>1.257293426477276</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.003738948847663</c:v>
+                  <c:v>1.222400729122967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.872427601237327</c:v>
+                  <c:v>0.887420063454305</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.156105752989131</c:v>
+                  <c:v>0.245178233209064</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.169043944507417</c:v>
+                  <c:v>0.178032784649426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,28 +781,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.284431423854797</c:v>
+                  <c:v>0.271306006662183</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.349390843046719</c:v>
+                  <c:v>0.32600305914484</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.399374817898374</c:v>
+                  <c:v>0.425084692310328</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.402640551670304</c:v>
+                  <c:v>0.50355943833737</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.424788958516393</c:v>
+                  <c:v>0.492810694779388</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.344452470173038</c:v>
+                  <c:v>0.527523287216489</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.340819797807574</c:v>
+                  <c:v>0.513645561437151</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.355805949088367</c:v>
+                  <c:v>0.48868308564711</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -892,28 +892,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.852033912887081</c:v>
+                  <c:v>0.809042445634184</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.038176003337939</c:v>
+                  <c:v>0.96629676110757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.080438674680863</c:v>
+                  <c:v>1.281051837309289</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.049063821005334</c:v>
+                  <c:v>1.27478348932973</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.049175878625608</c:v>
+                  <c:v>1.262233899579848</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.046010985152338</c:v>
+                  <c:v>1.174435044408559</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.999762500707314</c:v>
+                  <c:v>1.194873313783339</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.045313091138769</c:v>
+                  <c:v>1.191314771221277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1003,28 +1003,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.307168023906172</c:v>
+                  <c:v>0.292415494270463</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60884012905642</c:v>
+                  <c:v>0.579981512648424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.196535407124075</c:v>
+                  <c:v>1.402367544421127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.191741314715364</c:v>
+                  <c:v>2.689067186635368</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.104777476510881</c:v>
+                  <c:v>3.948304739361191</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.904092816938557</c:v>
+                  <c:v>4.56337816416914</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.795932252469243</c:v>
+                  <c:v>4.598726440843054</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.184074917611348</c:v>
+                  <c:v>4.679683544791367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1114,28 +1114,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.374654057415405</c:v>
+                  <c:v>0.35759771534249</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.717522907890303</c:v>
+                  <c:v>0.688261820495227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.397744200985185</c:v>
+                  <c:v>1.650554604668589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.947582865090537</c:v>
+                  <c:v>3.486015664212935</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.648690076688352</c:v>
+                  <c:v>4.341011729030183</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.03077262650442</c:v>
+                  <c:v>4.818437329236431</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.941210937269833</c:v>
+                  <c:v>4.732212285825153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.201387560876963</c:v>
+                  <c:v>4.725804539136027</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9073,63 +9073,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Insert Bandwidth</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -9205,28 +9149,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.850672355576037</c:v>
+                  <c:v>0.817434894795387</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.037487483379165</c:v>
+                  <c:v>0.981897436270829</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.051806915558913</c:v>
+                  <c:v>1.171880349024415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.970587686437515</c:v>
+                  <c:v>1.257293426477276</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.003738948847663</c:v>
+                  <c:v>1.222400729122967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.872427601237327</c:v>
+                  <c:v>0.887420063454305</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.156105752989131</c:v>
+                  <c:v>0.245178233209064</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.169043944507417</c:v>
+                  <c:v>0.178032784649426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9308,28 +9252,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.374654057415405</c:v>
+                  <c:v>0.35759771534249</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.717522907890303</c:v>
+                  <c:v>0.688261820495227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.397744200985185</c:v>
+                  <c:v>1.650554604668589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.947582865090537</c:v>
+                  <c:v>3.486015664212935</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.648690076688352</c:v>
+                  <c:v>4.341011729030183</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.03077262650442</c:v>
+                  <c:v>4.818437329236431</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.941210937269833</c:v>
+                  <c:v>4.732212285825153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.201387560876963</c:v>
+                  <c:v>4.725804539136027</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -33400,10 +33344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D32" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33416,14 +33360,15 @@
     <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="10" t="s">
@@ -33435,7 +33380,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -33461,215 +33406,215 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>13475923</v>
+        <v>139860298</v>
       </c>
       <c r="D5">
-        <v>4484332</v>
+        <v>46666680</v>
       </c>
       <c r="E5">
-        <v>13411659</v>
+        <v>140604969</v>
       </c>
       <c r="F5">
-        <v>4477166</v>
+        <v>47150768</v>
       </c>
       <c r="G5">
-        <v>12418927</v>
+        <v>130454690</v>
       </c>
       <c r="H5">
-        <v>10181919</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106675661</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>21052204</v>
+        <v>215079077</v>
       </c>
       <c r="D6">
-        <v>7353722</v>
+        <v>77700524</v>
       </c>
       <c r="E6">
-        <v>21836275</v>
+        <v>234028311</v>
       </c>
       <c r="F6">
-        <v>7348845</v>
+        <v>78954984</v>
       </c>
       <c r="G6">
-        <v>12531031</v>
+        <v>131545478</v>
       </c>
       <c r="H6">
-        <v>10632963</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>110850178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>37259617</v>
+        <v>381778362</v>
       </c>
       <c r="D7">
-        <v>14507215</v>
+        <v>130207739</v>
       </c>
       <c r="E7">
-        <v>38206688</v>
+        <v>358958799</v>
       </c>
       <c r="F7">
-        <v>14122772</v>
+        <v>119111410</v>
       </c>
       <c r="G7">
-        <v>12752476</v>
+        <v>108807346</v>
       </c>
       <c r="H7">
-        <v>10916725</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92446436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>73732728</v>
+        <v>569650624</v>
       </c>
       <c r="D8">
-        <v>31442371</v>
+        <v>242724391</v>
       </c>
       <c r="E8">
-        <v>75793603</v>
+        <v>606037258</v>
       </c>
       <c r="F8">
-        <v>29090297</v>
+        <v>239394206</v>
       </c>
       <c r="G8">
-        <v>13923896</v>
+        <v>113487600</v>
       </c>
       <c r="H8">
-        <v>10353425</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87542860</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B9">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>137188659</v>
+        <v>1131332869</v>
       </c>
       <c r="D9">
-        <v>60807799</v>
+        <v>499305627</v>
       </c>
       <c r="E9">
-        <v>143683481</v>
+        <v>1238511195</v>
       </c>
       <c r="F9">
-        <v>58174380</v>
+        <v>483548701</v>
       </c>
       <c r="G9">
-        <v>19658464</v>
+        <v>154585728</v>
       </c>
       <c r="H9">
-        <v>16727964</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>140601224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B10">
         <v>32</v>
       </c>
       <c r="C10">
-        <v>280203421</v>
+        <v>2409237788</v>
       </c>
       <c r="D10">
-        <v>139920278</v>
+        <v>1375564037</v>
       </c>
       <c r="E10">
-        <v>354389424</v>
+        <v>2314026991</v>
       </c>
       <c r="F10">
-        <v>116700794</v>
+        <v>1039396032</v>
       </c>
       <c r="G10">
-        <v>31267267</v>
+        <v>267499883</v>
       </c>
       <c r="H10">
-        <v>30284594</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>253340044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B11">
         <v>64</v>
       </c>
       <c r="C11">
-        <v>1602586792</v>
+        <v>10502470085</v>
       </c>
       <c r="D11">
-        <v>1563943803</v>
+        <v>9957679432</v>
       </c>
       <c r="E11">
-        <v>716333460</v>
+        <v>4753095195</v>
       </c>
       <c r="F11">
-        <v>244198622</v>
+        <v>2043234393</v>
       </c>
       <c r="G11">
-        <v>64316381</v>
+        <v>530887471</v>
       </c>
       <c r="H11">
-        <v>61945587</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>515912242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B12">
         <v>128</v>
       </c>
       <c r="C12">
-        <v>2846732926</v>
+        <v>28188926671</v>
       </c>
       <c r="D12">
-        <v>2888487082</v>
+        <v>27426479396</v>
       </c>
       <c r="E12">
-        <v>1372324581</v>
+        <v>9991777173</v>
       </c>
       <c r="F12">
-        <v>467114833</v>
+        <v>4098675361</v>
       </c>
       <c r="G12">
-        <v>116699930</v>
+        <v>1043406558</v>
       </c>
       <c r="H12">
-        <v>116219045</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1033223541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="10" t="s">
@@ -33681,7 +33626,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="str">
         <f>A4</f>
         <v>rows</v>
@@ -33715,279 +33660,279 @@
         <v>row store (inlined row insert)</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f t="shared" ref="A16:B23" si="1">A5</f>
-        <v>1000000</v>
+        <f>A5</f>
+        <v>10000000</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f>B5</f>
         <v>1</v>
       </c>
       <c r="C16" s="4">
         <f>C5*NUMBERS!$C$3</f>
-        <v>13.475923</v>
+        <v>139.860298</v>
       </c>
       <c r="D16" s="4">
         <f>D5*NUMBERS!$C$3</f>
-        <v>4.4843320000000002</v>
+        <v>46.666679999999999</v>
       </c>
       <c r="E16" s="4">
         <f>E5*NUMBERS!$C$3</f>
-        <v>13.411659</v>
+        <v>140.60496899999998</v>
       </c>
       <c r="F16" s="4">
         <f>F5*NUMBERS!$C$3</f>
-        <v>4.4771659999999995</v>
+        <v>47.150767999999999</v>
       </c>
       <c r="G16" s="4">
         <f>G5*NUMBERS!$C$3</f>
-        <v>12.418927</v>
+        <v>130.45469</v>
       </c>
       <c r="H16" s="4">
         <f>H5*NUMBERS!$C$3</f>
-        <v>10.181918999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106.67566099999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A6</f>
+        <v>10000000</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>2</v>
       </c>
       <c r="C17" s="4">
         <f>C6*NUMBERS!$C$3</f>
-        <v>21.052204</v>
+        <v>215.07907699999998</v>
       </c>
       <c r="D17" s="4">
         <f>D6*NUMBERS!$C$3</f>
-        <v>7.3537219999999994</v>
+        <v>77.700524000000001</v>
       </c>
       <c r="E17" s="4">
         <f>E6*NUMBERS!$C$3</f>
-        <v>21.836275000000001</v>
+        <v>234.028311</v>
       </c>
       <c r="F17" s="4">
         <f>F6*NUMBERS!$C$3</f>
-        <v>7.3488449999999998</v>
+        <v>78.954983999999996</v>
       </c>
       <c r="G17" s="4">
         <f>G6*NUMBERS!$C$3</f>
-        <v>12.531030999999999</v>
+        <v>131.545478</v>
       </c>
       <c r="H17" s="4">
         <f>H6*NUMBERS!$C$3</f>
-        <v>10.632963</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>110.850178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A7</f>
+        <v>10000000</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f>B7</f>
         <v>4</v>
       </c>
       <c r="C18" s="4">
         <f>C7*NUMBERS!$C$3</f>
-        <v>37.259616999999999</v>
+        <v>381.77836199999996</v>
       </c>
       <c r="D18" s="4">
         <f>D7*NUMBERS!$C$3</f>
-        <v>14.507214999999999</v>
+        <v>130.207739</v>
       </c>
       <c r="E18" s="4">
         <f>E7*NUMBERS!$C$3</f>
-        <v>38.206688</v>
+        <v>358.958799</v>
       </c>
       <c r="F18" s="4">
         <f>F7*NUMBERS!$C$3</f>
-        <v>14.122771999999999</v>
+        <v>119.11140999999999</v>
       </c>
       <c r="G18" s="4">
         <f>G7*NUMBERS!$C$3</f>
-        <v>12.752476</v>
+        <v>108.807346</v>
       </c>
       <c r="H18" s="4">
         <f>H7*NUMBERS!$C$3</f>
-        <v>10.916725</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92.446435999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A8</f>
+        <v>10000000</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f>B8</f>
         <v>8</v>
       </c>
       <c r="C19" s="4">
         <f>C8*NUMBERS!$C$3</f>
-        <v>73.732727999999994</v>
+        <v>569.65062399999999</v>
       </c>
       <c r="D19" s="4">
         <f>D8*NUMBERS!$C$3</f>
-        <v>31.442370999999998</v>
+        <v>242.724391</v>
       </c>
       <c r="E19" s="4">
         <f>E8*NUMBERS!$C$3</f>
-        <v>75.79360299999999</v>
+        <v>606.03725799999995</v>
       </c>
       <c r="F19" s="4">
         <f>F8*NUMBERS!$C$3</f>
-        <v>29.090297</v>
+        <v>239.394206</v>
       </c>
       <c r="G19" s="4">
         <f>G8*NUMBERS!$C$3</f>
-        <v>13.923895999999999</v>
+        <v>113.4876</v>
       </c>
       <c r="H19" s="4">
         <f>H8*NUMBERS!$C$3</f>
-        <v>10.353425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87.54285999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A9</f>
+        <v>10000000</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f>B9</f>
         <v>16</v>
       </c>
       <c r="C20" s="4">
         <f>C9*NUMBERS!$C$3</f>
-        <v>137.188659</v>
+        <v>1131.3328689999998</v>
       </c>
       <c r="D20" s="4">
         <f>D9*NUMBERS!$C$3</f>
-        <v>60.807798999999996</v>
+        <v>499.30562699999996</v>
       </c>
       <c r="E20" s="4">
         <f>E9*NUMBERS!$C$3</f>
-        <v>143.683481</v>
+        <v>1238.511195</v>
       </c>
       <c r="F20" s="4">
         <f>F9*NUMBERS!$C$3</f>
-        <v>58.174379999999999</v>
+        <v>483.54870099999999</v>
       </c>
       <c r="G20" s="4">
         <f>G9*NUMBERS!$C$3</f>
-        <v>19.658463999999999</v>
+        <v>154.58572799999999</v>
       </c>
       <c r="H20" s="4">
         <f>H9*NUMBERS!$C$3</f>
-        <v>16.727964</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>140.601224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A10</f>
+        <v>10000000</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f>B10</f>
         <v>32</v>
       </c>
       <c r="C21" s="4">
         <f>C10*NUMBERS!$C$3</f>
-        <v>280.20342099999999</v>
+        <v>2409.2377879999999</v>
       </c>
       <c r="D21" s="4">
         <f>D10*NUMBERS!$C$3</f>
-        <v>139.920278</v>
+        <v>1375.5640369999999</v>
       </c>
       <c r="E21" s="4">
         <f>E10*NUMBERS!$C$3</f>
-        <v>354.38942399999996</v>
+        <v>2314.0269909999997</v>
       </c>
       <c r="F21" s="4">
         <f>F10*NUMBERS!$C$3</f>
-        <v>116.70079399999999</v>
+        <v>1039.3960319999999</v>
       </c>
       <c r="G21" s="4">
         <f>G10*NUMBERS!$C$3</f>
-        <v>31.267266999999997</v>
+        <v>267.49988300000001</v>
       </c>
       <c r="H21" s="4">
         <f>H10*NUMBERS!$C$3</f>
-        <v>30.284593999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>253.34004399999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A11</f>
+        <v>10000000</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f>B11</f>
         <v>64</v>
       </c>
       <c r="C22" s="4">
         <f>C11*NUMBERS!$C$3</f>
-        <v>1602.5867919999998</v>
+        <v>10502.470084999999</v>
       </c>
       <c r="D22" s="4">
         <f>D11*NUMBERS!$C$3</f>
-        <v>1563.9438029999999</v>
+        <v>9957.679431999999</v>
       </c>
       <c r="E22" s="4">
         <f>E11*NUMBERS!$C$3</f>
-        <v>716.33345999999995</v>
+        <v>4753.0951949999999</v>
       </c>
       <c r="F22" s="4">
         <f>F11*NUMBERS!$C$3</f>
-        <v>244.198622</v>
+        <v>2043.234393</v>
       </c>
       <c r="G22" s="4">
         <f>G11*NUMBERS!$C$3</f>
-        <v>64.316380999999993</v>
+        <v>530.88747100000001</v>
       </c>
       <c r="H22" s="4">
         <f>H11*NUMBERS!$C$3</f>
-        <v>61.945586999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>515.91224199999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
+        <f>A12</f>
+        <v>10000000</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f>B12</f>
         <v>128</v>
       </c>
       <c r="C23" s="4">
         <f>C12*NUMBERS!$C$3</f>
-        <v>2846.7329259999997</v>
+        <v>28188.926670999997</v>
       </c>
       <c r="D23" s="4">
         <f>D12*NUMBERS!$C$3</f>
-        <v>2888.4870819999996</v>
+        <v>27426.479395999999</v>
       </c>
       <c r="E23" s="4">
         <f>E12*NUMBERS!$C$3</f>
-        <v>1372.3245809999999</v>
+        <v>9991.7771730000004</v>
       </c>
       <c r="F23" s="4">
         <f>F12*NUMBERS!$C$3</f>
-        <v>467.11483299999998</v>
+        <v>4098.6753609999996</v>
       </c>
       <c r="G23" s="4">
         <f>G12*NUMBERS!$C$3</f>
-        <v>116.69992999999999</v>
+        <v>1043.4065579999999</v>
       </c>
       <c r="H23" s="4">
         <f>H12*NUMBERS!$C$3</f>
-        <v>116.21904499999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1033.2235409999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="10" t="s">
@@ -33999,310 +33944,522 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="str">
         <f>A4</f>
         <v>rows</v>
       </c>
       <c r="B26" s="3" t="str">
-        <f t="shared" ref="B26:H26" si="2">B4</f>
+        <f t="shared" ref="B26:H26" si="1">B4</f>
         <v>columns</v>
       </c>
       <c r="C26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>col store (by field)</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>col store (inlined)</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>row store (by field)</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>row store (inlined)</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>row store (row insert)</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>row store (inlined row insert)</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f t="shared" ref="A27:B27" si="3">A5</f>
-        <v>1000000</v>
+        <f>A5</f>
+        <v>10000000</v>
       </c>
       <c r="B27">
-        <f t="shared" si="3"/>
+        <f>B5</f>
         <v>1</v>
       </c>
       <c r="C27" s="2">
         <f>$A27*$B27*NUMBERS!$C$2/C5*NUMBERS!$C$4</f>
-        <v>0.28307502689240654</v>
+        <v>0.27275054609314503</v>
       </c>
       <c r="D27" s="2">
         <f>$A27*$B27*NUMBERS!$C$2/D5*NUMBERS!$C$4</f>
-        <v>0.85067235557603682</v>
+        <v>0.81743489479538722</v>
       </c>
       <c r="E27" s="2">
         <f>$A27*$B27*NUMBERS!$C$2/E5*NUMBERS!$C$4</f>
-        <v>0.28443142385479681</v>
+        <v>0.27130600666218274</v>
       </c>
       <c r="F27" s="2">
         <f>$A27*$B27*NUMBERS!$C$2/F5*NUMBERS!$C$4</f>
-        <v>0.85203391288708086</v>
+        <v>0.80904244563418359</v>
       </c>
       <c r="G27" s="2">
         <f>$A27*$B27*NUMBERS!$C$2/G5*NUMBERS!$C$4</f>
-        <v>0.30716802390617159</v>
+        <v>0.29241549427046276</v>
       </c>
       <c r="H27" s="2">
         <f>$A27*$B27*NUMBERS!$C$2/H5*NUMBERS!$C$4</f>
-        <v>0.3746540574154047</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.35759771534249035</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f t="shared" ref="A28:B28" si="4">A6</f>
-        <v>1000000</v>
+        <f>A6</f>
+        <v>10000000</v>
       </c>
       <c r="B28">
-        <f t="shared" si="4"/>
+        <f>B6</f>
         <v>2</v>
       </c>
       <c r="C28" s="2">
         <f>$A28*$B28*NUMBERS!$C$2/C6*NUMBERS!$C$4</f>
-        <v>0.36240360065150423</v>
+        <v>0.35472509170429445</v>
       </c>
       <c r="D28" s="2">
         <f>$A28*$B28*NUMBERS!$C$2/D6*NUMBERS!$C$4</f>
-        <v>1.037487483379165</v>
+        <v>0.98189743627082871</v>
       </c>
       <c r="E28" s="2">
         <f>$A28*$B28*NUMBERS!$C$2/E6*NUMBERS!$C$4</f>
-        <v>0.3493908430467193</v>
+        <v>0.32600305914483996</v>
       </c>
       <c r="F28" s="2">
         <f>$A28*$B28*NUMBERS!$C$2/F6*NUMBERS!$C$4</f>
-        <v>1.0381760033379395</v>
+        <v>0.96629676110756979</v>
       </c>
       <c r="G28" s="2">
         <f>$A28*$B28*NUMBERS!$C$2/G6*NUMBERS!$C$4</f>
-        <v>0.60884012905642004</v>
+        <v>0.57998151264842412</v>
       </c>
       <c r="H28" s="2">
         <f>$A28*$B28*NUMBERS!$C$2/H6*NUMBERS!$C$4</f>
-        <v>0.71752290789030293</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.68826182049522733</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f t="shared" ref="A29:B29" si="5">A7</f>
-        <v>1000000</v>
+        <f>A7</f>
+        <v>10000000</v>
       </c>
       <c r="B29">
-        <f t="shared" si="5"/>
+        <f>B7</f>
         <v>4</v>
       </c>
       <c r="C29" s="2">
         <f>$A29*$B29*NUMBERS!$C$2/C7*NUMBERS!$C$4</f>
-        <v>0.40952619192247736</v>
+        <v>0.39967663391305558</v>
       </c>
       <c r="D29" s="2">
         <f>$A29*$B29*NUMBERS!$C$2/D7*NUMBERS!$C$4</f>
-        <v>1.0518069155589131</v>
+        <v>1.1718803490244154</v>
       </c>
       <c r="E29" s="2">
         <f>$A29*$B29*NUMBERS!$C$2/E7*NUMBERS!$C$4</f>
-        <v>0.3993748178983742</v>
+        <v>0.4250846923103283</v>
       </c>
       <c r="F29" s="2">
         <f>$A29*$B29*NUMBERS!$C$2/F7*NUMBERS!$C$4</f>
-        <v>1.0804386746808627</v>
+        <v>1.2810518373092887</v>
       </c>
       <c r="G29" s="2">
         <f>$A29*$B29*NUMBERS!$C$2/G7*NUMBERS!$C$4</f>
-        <v>1.1965354071240755</v>
+        <v>1.4023675444211274</v>
       </c>
       <c r="H29" s="2">
         <f>$A29*$B29*NUMBERS!$C$2/H7*NUMBERS!$C$4</f>
-        <v>1.3977442009851855</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.6505546046685888</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f t="shared" ref="A30:B30" si="6">A8</f>
-        <v>1000000</v>
+        <f>A8</f>
+        <v>10000000</v>
       </c>
       <c r="B30">
-        <f t="shared" si="6"/>
+        <f>B8</f>
         <v>8</v>
       </c>
       <c r="C30" s="2">
         <f>$A30*$B30*NUMBERS!$C$2/C8*NUMBERS!$C$4</f>
-        <v>0.41389460220432917</v>
+        <v>0.53572447460357731</v>
       </c>
       <c r="D30" s="2">
         <f>$A30*$B30*NUMBERS!$C$2/D8*NUMBERS!$C$4</f>
-        <v>0.97058768643751459</v>
+        <v>1.2572934264772757</v>
       </c>
       <c r="E30" s="2">
         <f>$A30*$B30*NUMBERS!$C$2/E8*NUMBERS!$C$4</f>
-        <v>0.40264055167030394</v>
+        <v>0.50355943833737038</v>
       </c>
       <c r="F30" s="2">
         <f>$A30*$B30*NUMBERS!$C$2/F8*NUMBERS!$C$4</f>
-        <v>1.0490638210053338</v>
+        <v>1.2747834893297292</v>
       </c>
       <c r="G30" s="2">
         <f>$A30*$B30*NUMBERS!$C$2/G8*NUMBERS!$C$4</f>
-        <v>2.1917413147153639</v>
+        <v>2.6890671866353681</v>
       </c>
       <c r="H30" s="2">
         <f>$A30*$B30*NUMBERS!$C$2/H8*NUMBERS!$C$4</f>
-        <v>2.9475828650905376</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3.4860156642129354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f t="shared" ref="A31:B31" si="7">A9</f>
-        <v>1000000</v>
+        <f>A9</f>
+        <v>10000000</v>
       </c>
       <c r="B31">
-        <f t="shared" si="7"/>
+        <f>B9</f>
         <v>16</v>
       </c>
       <c r="C31" s="2">
         <f>$A31*$B31*NUMBERS!$C$2/C9*NUMBERS!$C$4</f>
-        <v>0.44489943042595087</v>
+        <v>0.53949777225114814</v>
       </c>
       <c r="D31" s="2">
         <f>$A31*$B31*NUMBERS!$C$2/D9*NUMBERS!$C$4</f>
-        <v>1.0037389488476633</v>
+        <v>1.2224007291229666</v>
       </c>
       <c r="E31" s="2">
         <f>$A31*$B31*NUMBERS!$C$2/E9*NUMBERS!$C$4</f>
-        <v>0.42478895851639337</v>
+        <v>0.49281069477938794</v>
       </c>
       <c r="F31" s="2">
         <f>$A31*$B31*NUMBERS!$C$2/F9*NUMBERS!$C$4</f>
-        <v>1.049175878625608</v>
+        <v>1.2622338995798481</v>
       </c>
       <c r="G31" s="2">
         <f>$A31*$B31*NUMBERS!$C$2/G9*NUMBERS!$C$4</f>
-        <v>3.1047774765108809</v>
+        <v>3.9483047393611912</v>
       </c>
       <c r="H31" s="2">
         <f>$A31*$B31*NUMBERS!$C$2/H9*NUMBERS!$C$4</f>
-        <v>3.6486900766883528</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.3410117290301828</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f t="shared" ref="A32:B32" si="8">A10</f>
-        <v>1000000</v>
+        <f>A10</f>
+        <v>10000000</v>
       </c>
       <c r="B32">
-        <f t="shared" si="8"/>
+        <f>B10</f>
         <v>32</v>
       </c>
       <c r="C32" s="2">
         <f>$A32*$B32*NUMBERS!$C$2/C10*NUMBERS!$C$4</f>
-        <v>0.43564890130302869</v>
+        <v>0.50667606621484718</v>
       </c>
       <c r="D32" s="2">
         <f>$A32*$B32*NUMBERS!$C$2/D10*NUMBERS!$C$4</f>
-        <v>0.87242760123732743</v>
+        <v>0.88742006345430502</v>
       </c>
       <c r="E32" s="2">
         <f>$A32*$B32*NUMBERS!$C$2/E10*NUMBERS!$C$4</f>
-        <v>0.34445247017303765</v>
+        <v>0.52752328721648856</v>
       </c>
       <c r="F32" s="2">
         <f>$A32*$B32*NUMBERS!$C$2/F10*NUMBERS!$C$4</f>
-        <v>1.0460109851523376</v>
+        <v>1.1744350444085589</v>
       </c>
       <c r="G32" s="2">
         <f>$A32*$B32*NUMBERS!$C$2/G10*NUMBERS!$C$4</f>
-        <v>3.9040928169385571</v>
+        <v>4.5633781641691407</v>
       </c>
       <c r="H32" s="2">
         <f>$A32*$B32*NUMBERS!$C$2/H10*NUMBERS!$C$4</f>
-        <v>4.0307726265044197</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.8184373292364313</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>A11</f>
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33" si="9">B11</f>
+        <f>B11</f>
         <v>64</v>
       </c>
       <c r="C33" s="2">
         <f>$A33*$B33*NUMBERS!$C$2/C11*NUMBERS!$C$4</f>
-        <v>0.15234159311603762</v>
+        <v>0.23246019557693412</v>
       </c>
       <c r="D33" s="2">
         <f>$A33*$B33*NUMBERS!$C$2/D11*NUMBERS!$C$4</f>
-        <v>0.1561057529891309</v>
+        <v>0.24517823320906443</v>
       </c>
       <c r="E33" s="2">
         <f>$A33*$B33*NUMBERS!$C$2/E11*NUMBERS!$C$4</f>
-        <v>0.34081979780757415</v>
+        <v>0.51364556143715112</v>
       </c>
       <c r="F33" s="2">
         <f>$A33*$B33*NUMBERS!$C$2/F11*NUMBERS!$C$4</f>
-        <v>0.99976250070731365</v>
+        <v>1.1948733137833394</v>
       </c>
       <c r="G33" s="2">
         <f>$A33*$B33*NUMBERS!$C$2/G11*NUMBERS!$C$4</f>
-        <v>3.7959322524692429</v>
+        <v>4.5987264408430546</v>
       </c>
       <c r="H33" s="2">
         <f>$A33*$B33*NUMBERS!$C$2/H11*NUMBERS!$C$4</f>
-        <v>3.9412109372698332</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.7322122858251534</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f t="shared" ref="A34:B34" si="10">A12</f>
-        <v>1000000</v>
+        <f>A12</f>
+        <v>10000000</v>
       </c>
       <c r="B34">
-        <f t="shared" si="10"/>
+        <f>B12</f>
         <v>128</v>
       </c>
       <c r="C34" s="2">
         <f>$A34*$B34*NUMBERS!$C$2/C12*NUMBERS!$C$4</f>
-        <v>0.17152337879693319</v>
+        <v>0.17321739692285992</v>
       </c>
       <c r="D34" s="2">
         <f>$A34*$B34*NUMBERS!$C$2/D12*NUMBERS!$C$4</f>
-        <v>0.16904394450741739</v>
+        <v>0.17803278464942646</v>
       </c>
       <c r="E34" s="2">
         <f>$A34*$B34*NUMBERS!$C$2/E12*NUMBERS!$C$4</f>
-        <v>0.3558059490883666</v>
+        <v>0.48868308564711022</v>
       </c>
       <c r="F34" s="2">
         <f>$A34*$B34*NUMBERS!$C$2/F12*NUMBERS!$C$4</f>
-        <v>1.0453130911387694</v>
+        <v>1.191314771221277</v>
       </c>
       <c r="G34" s="2">
         <f>$A34*$B34*NUMBERS!$C$2/G12*NUMBERS!$C$4</f>
-        <v>4.1840749176113476</v>
+        <v>4.6796835447913674</v>
       </c>
       <c r="H34" s="2">
         <f>$A34*$B34*NUMBERS!$C$2/H12*NUMBERS!$C$4</f>
-        <v>4.2013875608769631</v>
+        <v>4.7258045391360275</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R89" s="4"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>10000000</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>139860298</v>
+      </c>
+      <c r="D90">
+        <v>46666680</v>
+      </c>
+      <c r="E90">
+        <v>140604969</v>
+      </c>
+      <c r="F90">
+        <v>47150768</v>
+      </c>
+      <c r="G90">
+        <v>130454690</v>
+      </c>
+      <c r="H90">
+        <v>106675661</v>
+      </c>
+      <c r="R90" s="1"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>10000000</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91">
+        <v>215079077</v>
+      </c>
+      <c r="D91">
+        <v>77700524</v>
+      </c>
+      <c r="E91">
+        <v>234028311</v>
+      </c>
+      <c r="F91">
+        <v>78954984</v>
+      </c>
+      <c r="G91">
+        <v>131545478</v>
+      </c>
+      <c r="H91">
+        <v>110850178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>10000000</v>
+      </c>
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92">
+        <v>381778362</v>
+      </c>
+      <c r="D92">
+        <v>130207739</v>
+      </c>
+      <c r="E92">
+        <v>358958799</v>
+      </c>
+      <c r="F92">
+        <v>119111410</v>
+      </c>
+      <c r="G92">
+        <v>108807346</v>
+      </c>
+      <c r="H92">
+        <v>92446436</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>10000000</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="C93">
+        <v>569650624</v>
+      </c>
+      <c r="D93">
+        <v>242724391</v>
+      </c>
+      <c r="E93">
+        <v>606037258</v>
+      </c>
+      <c r="F93">
+        <v>239394206</v>
+      </c>
+      <c r="G93">
+        <v>113487600</v>
+      </c>
+      <c r="H93">
+        <v>87542860</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>10000000</v>
+      </c>
+      <c r="B94">
+        <v>16</v>
+      </c>
+      <c r="C94">
+        <v>1131332869</v>
+      </c>
+      <c r="D94">
+        <v>499305627</v>
+      </c>
+      <c r="E94">
+        <v>1238511195</v>
+      </c>
+      <c r="F94">
+        <v>483548701</v>
+      </c>
+      <c r="G94">
+        <v>154585728</v>
+      </c>
+      <c r="H94">
+        <v>140601224</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>10000000</v>
+      </c>
+      <c r="B95">
+        <v>32</v>
+      </c>
+      <c r="C95">
+        <v>2409237788</v>
+      </c>
+      <c r="D95">
+        <v>1375564037</v>
+      </c>
+      <c r="E95">
+        <v>2314026991</v>
+      </c>
+      <c r="F95">
+        <v>1039396032</v>
+      </c>
+      <c r="G95">
+        <v>267499883</v>
+      </c>
+      <c r="H95">
+        <v>253340044</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>10000000</v>
+      </c>
+      <c r="B96">
+        <v>64</v>
+      </c>
+      <c r="C96">
+        <v>10502470085</v>
+      </c>
+      <c r="D96">
+        <v>9957679432</v>
+      </c>
+      <c r="E96">
+        <v>4753095195</v>
+      </c>
+      <c r="F96">
+        <v>2043234393</v>
+      </c>
+      <c r="G96">
+        <v>530887471</v>
+      </c>
+      <c r="H96">
+        <v>515912242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>10000000</v>
+      </c>
+      <c r="B97">
+        <v>128</v>
+      </c>
+      <c r="C97">
+        <v>28188926671</v>
+      </c>
+      <c r="D97">
+        <v>27426479396</v>
+      </c>
+      <c r="E97">
+        <v>9991777173</v>
+      </c>
+      <c r="F97">
+        <v>4098675361</v>
+      </c>
+      <c r="G97">
+        <v>1043406558</v>
+      </c>
+      <c r="H97">
+        <v>1033223541</v>
       </c>
     </row>
   </sheetData>
@@ -36548,7 +36705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="81" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+    <sheetView zoomScale="81" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
       <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
@@ -45186,7 +45343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated diagram font sizes
</commit_message>
<xml_diff>
--- a/tests/results/vm-results.xlsx
+++ b/tests/results/vm-results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxklenk/dev/hpi/epic-battle-db/tests/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaswollowski/Git/epic-battle-db/tests/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="20180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="NUMBERS" sheetId="3" r:id="rId1"/>
@@ -375,8 +375,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -471,7 +471,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1157,11 +1157,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131616880"/>
-        <c:axId val="2131620112"/>
+        <c:axId val="-1762776656"/>
+        <c:axId val="-1676525984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131616880"/>
+        <c:axId val="-1762776656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,10 +1201,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131620112"/>
+        <c:crossAx val="-1676525984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1212,7 +1212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131620112"/>
+        <c:axId val="-1676525984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +1284,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1316,10 +1316,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131616880"/>
+        <c:crossAx val="-1762776656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1358,7 +1358,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1396,7 +1396,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1447,7 +1447,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1473,7 +1472,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1634,11 +1633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132154736"/>
-        <c:axId val="2132160272"/>
+        <c:axId val="-1676391216"/>
+        <c:axId val="-1676387456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132154736"/>
+        <c:axId val="-1676391216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +1669,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1696,7 +1694,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1734,10 +1732,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132160272"/>
+        <c:crossAx val="-1676387456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1745,7 +1743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132160272"/>
+        <c:axId val="-1676387456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1791,7 +1789,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1817,7 +1814,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1849,10 +1846,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132154736"/>
+        <c:crossAx val="-1676391216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1866,7 +1863,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1892,7 +1888,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1917,7 +1913,7 @@
       <a:pPr>
         <a:defRPr sz="1200"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1994,7 +1990,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3010,11 +3006,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106704976"/>
-        <c:axId val="2113684992"/>
+        <c:axId val="-1727234640"/>
+        <c:axId val="-1727232160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106704976"/>
+        <c:axId val="-1727234640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3054,10 +3050,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113684992"/>
+        <c:crossAx val="-1727232160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3065,7 +3061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113684992"/>
+        <c:axId val="-1727232160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,7 +3133,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3169,10 +3165,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106704976"/>
+        <c:crossAx val="-1727234640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3211,7 +3207,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -3249,7 +3245,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3675,11 +3671,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106623104"/>
-        <c:axId val="2113639856"/>
+        <c:axId val="-1727193264"/>
+        <c:axId val="-1727190272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106623104"/>
+        <c:axId val="-1727193264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3719,10 +3715,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113639856"/>
+        <c:crossAx val="-1727190272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3730,7 +3726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113639856"/>
+        <c:axId val="-1727190272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,10 +3810,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106623104"/>
+        <c:crossAx val="-1727193264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3856,7 +3852,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -3872,7 +3868,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3949,7 +3945,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4165,11 +4161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2113666528"/>
-        <c:axId val="2113669536"/>
+        <c:axId val="-1676336384"/>
+        <c:axId val="-1676333904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113666528"/>
+        <c:axId val="-1676336384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4209,10 +4205,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113669536"/>
+        <c:crossAx val="-1676333904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4220,7 +4216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113669536"/>
+        <c:axId val="-1676333904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4267,7 +4263,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4299,10 +4295,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113666528"/>
+        <c:crossAx val="-1676336384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4341,7 +4337,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -4379,7 +4375,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4430,6 +4426,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4455,7 +4452,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4713,11 +4710,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132256400"/>
-        <c:axId val="2132261952"/>
+        <c:axId val="-1727148816"/>
+        <c:axId val="-1727145056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132256400"/>
+        <c:axId val="-1727148816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4749,6 +4746,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4774,7 +4772,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4812,10 +4810,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132261952"/>
+        <c:crossAx val="-1727145056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4823,7 +4821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132261952"/>
+        <c:axId val="-1727145056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150.0"/>
@@ -4870,6 +4868,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4895,7 +4894,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4927,10 +4926,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132256400"/>
+        <c:crossAx val="-1727148816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4944,6 +4943,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4969,7 +4969,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4999,7 +4999,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5031,10 +5031,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0623935104275058"/>
+          <c:x val="0.0921809951081094"/>
           <c:y val="0.0702745033699578"/>
-          <c:w val="0.925131308646479"/>
-          <c:h val="0.750403561910054"/>
+          <c:w val="0.895343836593181"/>
+          <c:h val="0.68697315754118"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5570,11 +5570,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132303312"/>
-        <c:axId val="2132308832"/>
+        <c:axId val="-1727126688"/>
+        <c:axId val="-1727122928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132303312"/>
+        <c:axId val="-1727126688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5587,7 +5587,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5600,13 +5600,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Selectivity / # Columns</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.440790389571714"/>
+              <c:y val="0.912134214191439"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5620,7 +5627,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5632,7 +5639,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5658,7 +5665,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5670,10 +5677,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132308832"/>
+        <c:crossAx val="-1727122928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5681,7 +5688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132308832"/>
+        <c:axId val="-1727122928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5708,7 +5715,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5721,13 +5728,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>MB/ms</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00768708364152284"/>
+              <c:y val="0.442118346020985"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5741,7 +5755,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5753,7 +5767,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5773,7 +5787,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5785,10 +5799,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132303312"/>
+        <c:crossAx val="-1727126688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5802,7 +5816,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.616296874564953"/>
+          <c:y val="0.908906440498489"/>
+          <c:w val="0.255535986446521"/>
+          <c:h val="0.0416328302350344"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5816,7 +5839,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5828,7 +5851,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5851,9 +5874,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6424,11 +6447,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132344352"/>
-        <c:axId val="2132349904"/>
+        <c:axId val="-1675566016"/>
+        <c:axId val="-1675563536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132344352"/>
+        <c:axId val="-1675566016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6441,7 +6464,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6454,7 +6477,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Selectivity / # Columns</a:t>
                 </a:r>
               </a:p>
@@ -6474,7 +6497,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6486,7 +6509,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6512,7 +6535,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6524,10 +6547,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132349904"/>
+        <c:crossAx val="-1675563536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6535,7 +6558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132349904"/>
+        <c:axId val="-1675563536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6562,7 +6585,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6575,7 +6598,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>MB/ms</a:t>
                 </a:r>
               </a:p>
@@ -6595,7 +6618,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6607,7 +6630,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6627,7 +6650,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6639,10 +6662,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132344352"/>
+        <c:crossAx val="-1675566016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6656,7 +6679,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.384582687625855"/>
+          <c:y val="0.961751306476871"/>
+          <c:w val="0.230834624748289"/>
+          <c:h val="0.0382486935231294"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6670,7 +6702,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6682,7 +6714,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6705,9 +6737,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1600"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6758,6 +6790,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6783,7 +6816,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7247,11 +7280,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132380320"/>
-        <c:axId val="2132383472"/>
+        <c:axId val="-1675551776"/>
+        <c:axId val="-1675549200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132380320"/>
+        <c:axId val="-1675551776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7291,10 +7324,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132383472"/>
+        <c:crossAx val="-1675549200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7302,7 +7335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132383472"/>
+        <c:axId val="-1675549200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7348,6 +7381,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7373,7 +7407,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7405,10 +7439,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132380320"/>
+        <c:crossAx val="-1675551776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7447,7 +7481,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -7485,7 +7519,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7541,6 +7575,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7566,7 +7601,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8030,11 +8065,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132437376"/>
-        <c:axId val="2132440528"/>
+        <c:axId val="-1675527120"/>
+        <c:axId val="-1675524128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132437376"/>
+        <c:axId val="-1675527120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8074,10 +8109,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132440528"/>
+        <c:crossAx val="-1675524128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8085,7 +8120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132440528"/>
+        <c:axId val="-1675524128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8131,6 +8166,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8156,7 +8192,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8188,10 +8224,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132437376"/>
+        <c:crossAx val="-1675527120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8230,7 +8266,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -8268,7 +8304,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8345,7 +8381,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8809,11 +8845,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2113772960"/>
-        <c:axId val="2113776112"/>
+        <c:axId val="-1676265104"/>
+        <c:axId val="-1676262112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113772960"/>
+        <c:axId val="-1676265104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8853,10 +8889,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113776112"/>
+        <c:crossAx val="-1676262112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8864,7 +8900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113776112"/>
+        <c:axId val="-1676262112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8936,7 +8972,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8968,10 +9004,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113772960"/>
+        <c:crossAx val="-1676265104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9010,7 +9046,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -9048,7 +9084,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9295,11 +9331,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131724480"/>
-        <c:axId val="2131730000"/>
+        <c:axId val="-1676500880"/>
+        <c:axId val="-1676497760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131724480"/>
+        <c:axId val="-1676500880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9312,7 +9348,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9325,7 +9361,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t># Columns</a:t>
                 </a:r>
               </a:p>
@@ -9345,7 +9381,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9357,7 +9393,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9383,7 +9419,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9395,10 +9431,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131730000"/>
+        <c:crossAx val="-1676497760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9406,7 +9442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131730000"/>
+        <c:axId val="-1676497760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9433,7 +9469,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9446,7 +9482,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>MB/ms</a:t>
                 </a:r>
               </a:p>
@@ -9466,7 +9502,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9478,7 +9514,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9498,7 +9534,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9510,10 +9546,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131724480"/>
+        <c:crossAx val="-1676500880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9541,7 +9577,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -9553,7 +9589,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9576,9 +9612,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9660,7 +9696,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10124,11 +10160,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132496208"/>
-        <c:axId val="2132499360"/>
+        <c:axId val="-1676241920"/>
+        <c:axId val="-1676238928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132496208"/>
+        <c:axId val="-1676241920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10168,10 +10204,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132499360"/>
+        <c:crossAx val="-1676238928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10179,7 +10215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132499360"/>
+        <c:axId val="-1676238928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10251,7 +10287,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10283,10 +10319,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132496208"/>
+        <c:crossAx val="-1676241920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10325,7 +10361,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -10363,7 +10399,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10447,7 +10483,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10771,11 +10807,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132564432"/>
-        <c:axId val="2132570096"/>
+        <c:axId val="-1762734832"/>
+        <c:axId val="-1675481360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132564432"/>
+        <c:axId val="-1762734832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10833,7 +10869,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10871,10 +10907,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132570096"/>
+        <c:crossAx val="-1675481360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10882,7 +10918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132570096"/>
+        <c:axId val="-1675481360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10954,7 +10990,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10986,10 +11022,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132564432"/>
+        <c:crossAx val="-1762734832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11029,7 +11065,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11054,7 +11090,7 @@
       <a:pPr>
         <a:defRPr sz="1200"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11138,7 +11174,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11326,11 +11362,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106604560"/>
-        <c:axId val="2106653552"/>
+        <c:axId val="-1727080800"/>
+        <c:axId val="-1727077040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106604560"/>
+        <c:axId val="-1727080800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11388,7 +11424,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11426,10 +11462,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106653552"/>
+        <c:crossAx val="-1727077040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11437,7 +11473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106653552"/>
+        <c:axId val="-1727077040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11509,7 +11545,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11541,10 +11577,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106604560"/>
+        <c:crossAx val="-1727080800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11584,7 +11620,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11609,7 +11645,7 @@
       <a:pPr>
         <a:defRPr sz="1200"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11817,11 +11853,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2093243568"/>
-        <c:axId val="-2093230544"/>
+        <c:axId val="-1676211072"/>
+        <c:axId val="-1676207040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093243568"/>
+        <c:axId val="-1676211072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11834,7 +11870,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -11847,7 +11883,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t># Threads</a:t>
                 </a:r>
               </a:p>
@@ -11867,7 +11903,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -11879,10 +11915,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11904,7 +11941,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -11916,10 +11953,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093230544"/>
+        <c:crossAx val="-1676207040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11927,7 +11964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093230544"/>
+        <c:axId val="-1676207040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11954,7 +11991,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -11967,13 +12004,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>MB/ms</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00974025974025974"/>
+              <c:y val="0.354359651791877"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11987,7 +12031,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -11999,7 +12043,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12018,7 +12062,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -12030,10 +12074,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093243568"/>
+        <c:crossAx val="-1676211072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12061,7 +12105,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -12073,7 +12117,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12096,9 +12140,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12149,7 +12193,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12175,7 +12218,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12391,11 +12434,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2113845552"/>
-        <c:axId val="2113851072"/>
+        <c:axId val="-1727040672"/>
+        <c:axId val="-1727036912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113845552"/>
+        <c:axId val="-1727040672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12427,7 +12470,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12453,7 +12495,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12491,10 +12533,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113851072"/>
+        <c:crossAx val="-1727036912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12502,7 +12544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113851072"/>
+        <c:axId val="-1727036912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12548,7 +12590,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12574,7 +12615,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12606,10 +12647,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113845552"/>
+        <c:crossAx val="-1727040672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12623,7 +12664,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12649,7 +12689,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12674,7 +12714,7 @@
       <a:pPr>
         <a:defRPr sz="1200"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12788,16 +12828,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="2132629600"/>
-        <c:axId val="2132632864"/>
+        <c:axId val="-1675452608"/>
+        <c:axId val="-1675449856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2132629600"/>
+        <c:axId val="-1675452608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12831,10 +12872,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132632864"/>
+        <c:crossAx val="-1675449856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12842,7 +12883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132632864"/>
+        <c:axId val="-1675449856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12913,7 +12954,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12944,10 +12985,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132629600"/>
+        <c:crossAx val="-1675452608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12980,7 +13021,7 @@
       <a:pPr>
         <a:defRPr sz="1200"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13056,7 +13097,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13308,11 +13349,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131528144"/>
-        <c:axId val="2131578800"/>
+        <c:axId val="-1761634672"/>
+        <c:axId val="-1761632624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131528144"/>
+        <c:axId val="-1761634672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13352,10 +13393,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131578800"/>
+        <c:crossAx val="-1761632624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13363,7 +13404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131578800"/>
+        <c:axId val="-1761632624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13434,7 +13475,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13466,10 +13507,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131528144"/>
+        <c:crossAx val="-1761634672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13508,7 +13549,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -13546,7 +13587,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13622,7 +13663,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13864,11 +13905,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2130788400"/>
-        <c:axId val="2130785392"/>
+        <c:axId val="-1727339600"/>
+        <c:axId val="-1727337120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2130788400"/>
+        <c:axId val="-1727339600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13908,10 +13949,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130785392"/>
+        <c:crossAx val="-1727337120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13919,7 +13960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130785392"/>
+        <c:axId val="-1727337120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13990,7 +14031,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14022,10 +14063,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130788400"/>
+        <c:crossAx val="-1727339600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14064,7 +14105,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -14102,7 +14143,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14178,7 +14219,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -14936,11 +14977,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131907936"/>
-        <c:axId val="2131911072"/>
+        <c:axId val="-1676439024"/>
+        <c:axId val="-1676436544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131907936"/>
+        <c:axId val="-1676439024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14980,10 +15021,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131911072"/>
+        <c:crossAx val="-1676436544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14991,7 +15032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131911072"/>
+        <c:axId val="-1676436544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15062,7 +15103,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15094,10 +15135,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131907936"/>
+        <c:crossAx val="-1676439024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15136,7 +15177,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -15174,7 +15215,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15250,7 +15291,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -16008,11 +16049,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131957456"/>
-        <c:axId val="2131960672"/>
+        <c:axId val="-1727298880"/>
+        <c:axId val="-1727296400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131957456"/>
+        <c:axId val="-1727298880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16052,10 +16093,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131960672"/>
+        <c:crossAx val="-1727296400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16063,7 +16104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131960672"/>
+        <c:axId val="-1727296400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16134,7 +16175,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -16166,10 +16207,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131957456"/>
+        <c:crossAx val="-1727298880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16208,7 +16249,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -16246,7 +16287,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16322,7 +16363,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -16512,11 +16553,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131997792"/>
-        <c:axId val="2132003328"/>
+        <c:axId val="-1676423664"/>
+        <c:axId val="-1676419904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131997792"/>
+        <c:axId val="-1676423664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16573,7 +16614,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -16611,10 +16652,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132003328"/>
+        <c:crossAx val="-1676419904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16622,7 +16663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132003328"/>
+        <c:axId val="-1676419904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16693,7 +16734,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -16725,10 +16766,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131997792"/>
+        <c:crossAx val="-1676423664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16767,7 +16808,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -16792,7 +16833,7 @@
       <a:pPr>
         <a:defRPr sz="1200"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16843,7 +16884,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16869,7 +16909,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -17492,11 +17532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132077744"/>
-        <c:axId val="2132080832"/>
+        <c:axId val="-1675610784"/>
+        <c:axId val="-1675608720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132077744"/>
+        <c:axId val="-1675610784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17536,10 +17576,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132080832"/>
+        <c:crossAx val="-1675608720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17547,7 +17587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132080832"/>
+        <c:axId val="-1675608720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17593,7 +17633,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17619,7 +17658,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -17651,10 +17690,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132077744"/>
+        <c:crossAx val="-1675610784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17693,7 +17732,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -17731,7 +17770,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -17782,7 +17821,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17808,7 +17846,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -18431,11 +18469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132136832"/>
-        <c:axId val="2132139920"/>
+        <c:axId val="-1727270192"/>
+        <c:axId val="-1675593280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132136832"/>
+        <c:axId val="-1727270192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18475,10 +18513,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132139920"/>
+        <c:crossAx val="-1675593280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18486,7 +18524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132139920"/>
+        <c:axId val="-1675593280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18532,7 +18570,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18558,7 +18595,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -18590,10 +18627,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132136832"/>
+        <c:crossAx val="-1727270192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18632,7 +18669,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -18670,7 +18707,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -31735,7 +31772,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31771,7 +31808,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31849,7 +31886,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31885,7 +31922,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31928,7 +31965,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31966,7 +32003,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32004,7 +32041,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32047,7 +32084,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32085,7 +32122,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32123,7 +32160,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32166,7 +32203,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32202,7 +32239,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32240,7 +32277,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32278,7 +32315,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0B75F091-D886-4962-BE44-55A728CC26BA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B75F091-D886-4962-BE44-55A728CC26BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32301,13 +32338,13 @@
       <xdr:col>35</xdr:col>
       <xdr:colOff>788276</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>145977</xdr:rowOff>
+      <xdr:rowOff>145976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>709449</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>50509</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>172468</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32330,16 +32367,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>768272</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>47037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>767840</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>107732</xdr:rowOff>
+      <xdr:colOff>830556</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>154769</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32383,7 +32420,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32421,7 +32458,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32464,7 +32501,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32502,7 +32539,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32540,7 +32577,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32578,7 +32615,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33346,7 +33383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" workbookViewId="0">
+    <sheetView topLeftCell="H37" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:H12"/>
     </sheetView>
   </sheetViews>
@@ -33628,45 +33665,45 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="str">
-        <f>A4</f>
+        <f t="shared" ref="A15:B23" si="0">A4</f>
         <v>rows</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f>B4</f>
+        <f t="shared" si="0"/>
         <v>columns</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f t="shared" ref="C15:H15" si="0">C4</f>
+        <f t="shared" ref="C15:H15" si="1">C4</f>
         <v>col store (by field)</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>col store (inlined)</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>row store (by field)</v>
       </c>
       <c r="F15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>row store (inlined)</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>row store (row insert)</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>row store (inlined row insert)</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B16">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C16" s="4">
@@ -33696,11 +33733,11 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B17">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C17" s="4">
@@ -33730,11 +33767,11 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B18">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C18" s="4">
@@ -33764,11 +33801,11 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B19">
-        <f>B8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C19" s="4">
@@ -33798,11 +33835,11 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B20">
-        <f>B9</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C20" s="4">
@@ -33832,11 +33869,11 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B21">
-        <f>B10</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C21" s="4">
@@ -33866,11 +33903,11 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B22">
-        <f>B11</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="C22" s="4">
@@ -33900,11 +33937,11 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="B23">
-        <f>B12</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="C23" s="4">
@@ -33946,45 +33983,45 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="str">
-        <f>A4</f>
+        <f t="shared" ref="A26:A34" si="2">A4</f>
         <v>rows</v>
       </c>
       <c r="B26" s="3" t="str">
-        <f t="shared" ref="B26:H26" si="1">B4</f>
+        <f t="shared" ref="B26:H26" si="3">B4</f>
         <v>columns</v>
       </c>
       <c r="C26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>col store (by field)</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>col store (inlined)</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>row store (by field)</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>row store (inlined)</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>row store (row insert)</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>row store (inlined row insert)</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f>A5</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B27">
-        <f>B5</f>
+        <f t="shared" ref="B27:B34" si="4">B5</f>
         <v>1</v>
       </c>
       <c r="C27" s="2">
@@ -34014,11 +34051,11 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f>A6</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B28">
-        <f>B6</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="C28" s="2">
@@ -34048,11 +34085,11 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f>A7</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B29">
-        <f>B7</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="C29" s="2">
@@ -34082,11 +34119,11 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f>A8</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B30">
-        <f>B8</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="C30" s="2">
@@ -34116,11 +34153,11 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f>A9</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B31">
-        <f>B9</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="C31" s="2">
@@ -34150,11 +34187,11 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f>A10</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B32">
-        <f>B10</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="C32" s="2">
@@ -34184,11 +34221,11 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f>A11</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B33">
-        <f>B11</f>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="C33" s="2">
@@ -34218,11 +34255,11 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f>A12</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="B34">
-        <f>B12</f>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="C34" s="2">
@@ -36705,7 +36742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+    <sheetView topLeftCell="AG18" zoomScale="81" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
       <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
@@ -39792,7 +39829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C125" workbookViewId="0">
       <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
@@ -43103,7 +43140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
+    <sheetView topLeftCell="A104" zoomScale="99" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -45343,8 +45380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update update font size
</commit_message>
<xml_diff>
--- a/tests/results/vm-results.xlsx
+++ b/tests/results/vm-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NUMBERS" sheetId="3" r:id="rId1"/>
@@ -445,7 +445,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1157,11 +1156,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1762776656"/>
-        <c:axId val="-1676525984"/>
+        <c:axId val="-1651018848"/>
+        <c:axId val="-1651017216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1762776656"/>
+        <c:axId val="-1651018848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,7 +1203,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676525984"/>
+        <c:crossAx val="-1651017216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1212,7 +1211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676525984"/>
+        <c:axId val="-1651017216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1257,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1319,7 +1317,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1762776656"/>
+        <c:crossAx val="-1651018848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,62 +1419,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Update - Bandwidth</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1633,11 +1576,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676391216"/>
-        <c:axId val="-1676387456"/>
+        <c:axId val="-1536885888"/>
+        <c:axId val="-1536882768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676391216"/>
+        <c:axId val="-1536885888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1593,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1663,12 +1606,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t># Updated Columns</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1682,7 +1626,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1720,7 +1664,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1735,7 +1679,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676387456"/>
+        <c:crossAx val="-1536882768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1743,7 +1687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676387456"/>
+        <c:axId val="-1536882768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1714,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1783,12 +1727,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>MB/ms</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1802,7 +1747,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1834,7 +1779,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1849,7 +1794,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676391216"/>
+        <c:crossAx val="-1536885888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1863,6 +1808,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1876,7 +1822,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1911,7 +1857,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="de-DE"/>
     </a:p>
@@ -1964,7 +1910,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3006,11 +2951,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727234640"/>
-        <c:axId val="-1727232160"/>
+        <c:axId val="-1651051392"/>
+        <c:axId val="-1651049344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727234640"/>
+        <c:axId val="-1651051392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3053,7 +2998,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727232160"/>
+        <c:crossAx val="-1651049344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3061,7 +3006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727232160"/>
+        <c:axId val="-1651049344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3107,7 +3052,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3168,7 +3112,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727234640"/>
+        <c:crossAx val="-1651051392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3301,7 +3245,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3671,11 +3614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727193264"/>
-        <c:axId val="-1727190272"/>
+        <c:axId val="-1536959456"/>
+        <c:axId val="-1536220256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727193264"/>
+        <c:axId val="-1536959456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3718,7 +3661,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727190272"/>
+        <c:crossAx val="-1536220256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3726,7 +3669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727190272"/>
+        <c:axId val="-1536220256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3772,7 +3715,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3813,7 +3755,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727193264"/>
+        <c:crossAx val="-1536959456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3919,7 +3861,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4161,11 +4102,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676336384"/>
-        <c:axId val="-1676333904"/>
+        <c:axId val="-1537113952"/>
+        <c:axId val="-1537111904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676336384"/>
+        <c:axId val="-1537113952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4208,7 +4149,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676333904"/>
+        <c:crossAx val="-1537111904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4216,7 +4157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676333904"/>
+        <c:axId val="-1537111904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4237,7 +4178,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4298,7 +4238,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676336384"/>
+        <c:crossAx val="-1537113952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4426,7 +4366,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4710,11 +4649,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727148816"/>
-        <c:axId val="-1727145056"/>
+        <c:axId val="-1676405760"/>
+        <c:axId val="-1676402640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727148816"/>
+        <c:axId val="-1676405760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4746,7 +4685,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4813,7 +4751,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727145056"/>
+        <c:crossAx val="-1676402640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4821,7 +4759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727145056"/>
+        <c:axId val="-1676402640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150.0"/>
@@ -4868,7 +4806,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4929,7 +4866,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727148816"/>
+        <c:crossAx val="-1676405760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4943,7 +4880,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5570,11 +5506,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727126688"/>
-        <c:axId val="-1727122928"/>
+        <c:axId val="-1676471184"/>
+        <c:axId val="-1676468064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727126688"/>
+        <c:axId val="-1676471184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5680,7 +5616,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727122928"/>
+        <c:crossAx val="-1676468064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5688,7 +5624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727122928"/>
+        <c:axId val="-1676468064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5802,7 +5738,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727126688"/>
+        <c:crossAx val="-1676471184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6447,11 +6383,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1675566016"/>
-        <c:axId val="-1675563536"/>
+        <c:axId val="-1676441632"/>
+        <c:axId val="-1676438512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1675566016"/>
+        <c:axId val="-1676441632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6483,7 +6419,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6550,7 +6485,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675563536"/>
+        <c:crossAx val="-1676438512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6558,7 +6493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675563536"/>
+        <c:axId val="-1676438512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6604,7 +6539,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6665,7 +6599,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675566016"/>
+        <c:crossAx val="-1676441632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6790,7 +6724,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7280,11 +7213,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1675551776"/>
-        <c:axId val="-1675549200"/>
+        <c:axId val="-1676571488"/>
+        <c:axId val="-1676569344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1675551776"/>
+        <c:axId val="-1676571488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7327,7 +7260,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675549200"/>
+        <c:crossAx val="-1676569344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7335,7 +7268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675549200"/>
+        <c:axId val="-1676569344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7381,7 +7314,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7442,7 +7374,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675551776"/>
+        <c:crossAx val="-1676571488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7575,7 +7507,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8065,11 +7996,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1675527120"/>
-        <c:axId val="-1675524128"/>
+        <c:axId val="-1536267520"/>
+        <c:axId val="-1536996304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1675527120"/>
+        <c:axId val="-1536267520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8112,7 +8043,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675524128"/>
+        <c:crossAx val="-1536996304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8120,7 +8051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675524128"/>
+        <c:axId val="-1536996304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8166,7 +8097,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8227,7 +8157,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675527120"/>
+        <c:crossAx val="-1536267520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8355,7 +8285,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8845,11 +8774,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676265104"/>
-        <c:axId val="-1676262112"/>
+        <c:axId val="-1537032304"/>
+        <c:axId val="-1537030160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676265104"/>
+        <c:axId val="-1537032304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8892,7 +8821,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676262112"/>
+        <c:crossAx val="-1537030160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8900,7 +8829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676262112"/>
+        <c:axId val="-1537030160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8946,7 +8875,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9007,7 +8935,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676265104"/>
+        <c:crossAx val="-1537032304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9331,11 +9259,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676500880"/>
-        <c:axId val="-1676497760"/>
+        <c:axId val="-1674772288"/>
+        <c:axId val="-1674769584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676500880"/>
+        <c:axId val="-1674772288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9367,7 +9295,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9434,7 +9361,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676497760"/>
+        <c:crossAx val="-1674769584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9442,7 +9369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676497760"/>
+        <c:axId val="-1674769584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9488,7 +9415,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9549,7 +9475,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676500880"/>
+        <c:crossAx val="-1674772288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9563,7 +9489,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9670,7 +9595,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10160,11 +10084,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676241920"/>
-        <c:axId val="-1676238928"/>
+        <c:axId val="-1650814256"/>
+        <c:axId val="-1650812384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676241920"/>
+        <c:axId val="-1650814256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10207,7 +10131,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676238928"/>
+        <c:crossAx val="-1650812384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10215,7 +10139,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676238928"/>
+        <c:axId val="-1650812384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10261,7 +10185,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10322,7 +10245,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676241920"/>
+        <c:crossAx val="-1650814256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10807,11 +10730,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1762734832"/>
-        <c:axId val="-1675481360"/>
+        <c:axId val="-1651473616"/>
+        <c:axId val="-1651206288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1762734832"/>
+        <c:axId val="-1651473616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10843,7 +10766,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10910,7 +10832,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675481360"/>
+        <c:crossAx val="-1651206288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10918,7 +10840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675481360"/>
+        <c:axId val="-1651206288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10964,7 +10886,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11025,7 +10946,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1762734832"/>
+        <c:crossAx val="-1651473616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11039,7 +10960,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11362,11 +11282,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727080800"/>
-        <c:axId val="-1727077040"/>
+        <c:axId val="-1651135504"/>
+        <c:axId val="-1651077248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727080800"/>
+        <c:axId val="-1651135504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11398,7 +11318,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11465,7 +11384,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727077040"/>
+        <c:crossAx val="-1651077248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11473,7 +11392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727077040"/>
+        <c:axId val="-1651077248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11519,7 +11438,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11580,7 +11498,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727080800"/>
+        <c:crossAx val="-1651135504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11594,7 +11512,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11853,11 +11770,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1676211072"/>
-        <c:axId val="-1676207040"/>
+        <c:axId val="-1650879920"/>
+        <c:axId val="-1650876528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1676211072"/>
+        <c:axId val="-1650879920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11956,7 +11873,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676207040"/>
+        <c:crossAx val="-1650876528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11964,7 +11881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676207040"/>
+        <c:axId val="-1650876528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12077,7 +11994,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676211072"/>
+        <c:crossAx val="-1650879920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12434,11 +12351,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727040672"/>
-        <c:axId val="-1727036912"/>
+        <c:axId val="-1650925520"/>
+        <c:axId val="-1650927856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727040672"/>
+        <c:axId val="-1650925520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12536,7 +12453,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727036912"/>
+        <c:crossAx val="-1650927856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12544,7 +12461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727036912"/>
+        <c:axId val="-1650927856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12650,7 +12567,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727040672"/>
+        <c:crossAx val="-1650925520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12828,11 +12745,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-1675452608"/>
-        <c:axId val="-1675449856"/>
+        <c:axId val="-1537207520"/>
+        <c:axId val="-1537205744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1675452608"/>
+        <c:axId val="-1537207520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12875,7 +12792,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675449856"/>
+        <c:crossAx val="-1537205744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12883,7 +12800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675449856"/>
+        <c:axId val="-1537205744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12988,7 +12905,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675452608"/>
+        <c:crossAx val="-1537207520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13349,11 +13266,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1761634672"/>
-        <c:axId val="-1761632624"/>
+        <c:axId val="-1579435968"/>
+        <c:axId val="-1579434608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1761634672"/>
+        <c:axId val="-1579435968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13396,7 +13313,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1761632624"/>
+        <c:crossAx val="-1579434608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13404,7 +13321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1761632624"/>
+        <c:axId val="-1579434608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13510,7 +13427,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1761634672"/>
+        <c:crossAx val="-1579435968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13905,11 +13822,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727339600"/>
-        <c:axId val="-1727337120"/>
+        <c:axId val="-1542354112"/>
+        <c:axId val="-1542352752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727339600"/>
+        <c:axId val="-1542354112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13952,7 +13869,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727337120"/>
+        <c:crossAx val="-1542352752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13960,7 +13877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727337120"/>
+        <c:axId val="-1542352752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14066,7 +13983,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727339600"/>
+        <c:crossAx val="-1542354112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14194,6 +14111,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14977,11 +14895,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676439024"/>
-        <c:axId val="-1676436544"/>
+        <c:axId val="-1651101456"/>
+        <c:axId val="-1650979664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676439024"/>
+        <c:axId val="-1651101456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15024,7 +14942,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676436544"/>
+        <c:crossAx val="-1650979664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15032,7 +14950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676436544"/>
+        <c:axId val="-1650979664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15078,6 +14996,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15138,7 +15057,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676439024"/>
+        <c:crossAx val="-1651101456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15266,6 +15185,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16049,11 +15969,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727298880"/>
-        <c:axId val="-1727296400"/>
+        <c:axId val="-1650852896"/>
+        <c:axId val="-1650851536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727298880"/>
+        <c:axId val="-1650852896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16096,7 +16016,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727296400"/>
+        <c:crossAx val="-1650851536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16104,7 +16024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727296400"/>
+        <c:axId val="-1650851536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16150,6 +16070,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16210,7 +16131,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727298880"/>
+        <c:crossAx val="-1650852896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16338,6 +16259,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16553,11 +16475,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1676423664"/>
-        <c:axId val="-1676419904"/>
+        <c:axId val="-1536688928"/>
+        <c:axId val="-1536686800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1676423664"/>
+        <c:axId val="-1536688928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16589,6 +16511,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16655,7 +16578,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676419904"/>
+        <c:crossAx val="-1536686800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16663,7 +16586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676419904"/>
+        <c:axId val="-1536686800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16709,6 +16632,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16769,7 +16693,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676423664"/>
+        <c:crossAx val="-1536688928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16783,6 +16707,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16884,6 +16809,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17532,11 +17458,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1675610784"/>
-        <c:axId val="-1675608720"/>
+        <c:axId val="-1536604480"/>
+        <c:axId val="-1536602848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1675610784"/>
+        <c:axId val="-1536604480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17579,7 +17505,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675608720"/>
+        <c:crossAx val="-1536602848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17587,7 +17513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675608720"/>
+        <c:axId val="-1536602848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17633,6 +17559,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17693,7 +17620,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675610784"/>
+        <c:crossAx val="-1536604480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17821,6 +17748,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18469,11 +18397,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1727270192"/>
-        <c:axId val="-1675593280"/>
+        <c:axId val="-1542311008"/>
+        <c:axId val="-1542153728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1727270192"/>
+        <c:axId val="-1542311008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18516,7 +18444,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1675593280"/>
+        <c:crossAx val="-1542153728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18524,7 +18452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1675593280"/>
+        <c:axId val="-1542153728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18570,6 +18498,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18630,7 +18559,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727270192"/>
+        <c:crossAx val="-1542311008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -31772,7 +31701,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31808,7 +31737,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31886,7 +31815,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31922,7 +31851,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31965,7 +31894,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32003,7 +31932,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32041,7 +31970,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32084,7 +32013,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32122,7 +32051,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32144,23 +32073,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>21167</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>46567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>21167</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32203,7 +32132,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32239,7 +32168,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32277,7 +32206,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32315,7 +32244,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B75F091-D886-4962-BE44-55A728CC26BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0B75F091-D886-4962-BE44-55A728CC26BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32420,7 +32349,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32458,7 +32387,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32501,7 +32430,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32539,7 +32468,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32577,7 +32506,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32615,7 +32544,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35846,8 +35775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="109" workbookViewId="0">
-      <selection activeCell="W77" sqref="W77"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="50" workbookViewId="0">
+      <selection activeCell="AA81" sqref="AA81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45380,7 +45309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>

</xml_diff>